<commit_message>
example untill 4116K v0
</commit_message>
<xml_diff>
--- a/Abbr-RSC current journals_NT.xlsx
+++ b/Abbr-RSC current journals_NT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>an</t>
   </si>
@@ -291,10 +291,22 @@
     <t xml:space="preserve">Toxicology Research </t>
   </si>
   <si>
-    <t>Publisher: Royal Society of Chemistry</t>
-  </si>
-  <si>
     <t>Jounal name</t>
+  </si>
+  <si>
+    <t>ISSN(online)</t>
+  </si>
+  <si>
+    <t>ISSN(print)</t>
+  </si>
+  <si>
+    <t>1463-9084</t>
+  </si>
+  <si>
+    <t>1463-9076</t>
+  </si>
+  <si>
+    <t>Publisher: The Royal Society of Chemistry</t>
   </si>
 </sst>
 </file>
@@ -651,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,21 +677,27 @@
     <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B1" s="4"/>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -687,7 +705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -695,7 +713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -703,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -711,7 +729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -719,7 +737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -727,7 +745,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -735,7 +753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -743,7 +761,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -751,7 +769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -759,7 +777,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -767,7 +785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -775,7 +793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -783,7 +801,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -919,7 +937,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -927,7 +945,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -935,7 +953,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -943,7 +961,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -951,7 +969,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -959,7 +977,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -967,7 +985,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -975,7 +993,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -983,15 +1001,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>84</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -999,7 +1023,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -1007,7 +1031,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -1015,7 +1039,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -1023,7 +1047,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>89</v>
       </c>
@@ -1031,7 +1055,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
updates untill 04116k -v1
</commit_message>
<xml_diff>
--- a/Abbr-RSC current journals_NT.xlsx
+++ b/Abbr-RSC current journals_NT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>an</t>
   </si>
@@ -307,6 +307,18 @@
   </si>
   <si>
     <t>Publisher: The Royal Society of Chemistry</t>
+  </si>
+  <si>
+    <t>1477-0520</t>
+  </si>
+  <si>
+    <t>1477-0539</t>
+  </si>
+  <si>
+    <t>2041-6539</t>
+  </si>
+  <si>
+    <t>1466-8033</t>
   </si>
 </sst>
 </file>
@@ -666,7 +678,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,6 +756,9 @@
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D8" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -768,6 +783,9 @@
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="D11" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -983,6 +1001,12 @@
       </c>
       <c r="B38" s="3" t="s">
         <v>35</v>
+      </c>
+      <c r="C38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>